<commit_message>
Adapt model interface for addition of lever starts and ends
</commit_message>
<xml_diff>
--- a/tests/test_model/test.xlsx
+++ b/tests/test_model/test.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccaveayl\vmware_shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204F304D-B39A-48AC-BA0A-C53989C89575}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A1CA23-C9CB-44C8-9CDE-ABCEEAA433C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E3E7D5AE-718D-4492-A5CF-364461443CE4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Control" sheetId="3" r:id="rId2"/>
-    <sheet name="WebOutputs" sheetId="2" r:id="rId3"/>
+    <sheet name="Control" sheetId="2" r:id="rId2"/>
+    <sheet name="WebOutputs" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="INPUT.FACTOR">Control!$B$1</definedName>
     <definedName name="input.lever.ambition">Control!$B$1:$B$2</definedName>
+    <definedName name="input.lever.end">Control!$D$1:$D$2</definedName>
+    <definedName name="input.lever.start">Control!$C$1:$C$2</definedName>
     <definedName name="INPUT.OFFSET">Control!$B$2</definedName>
     <definedName name="OUTPUT.a">Sheet1!$A$2:$U$2</definedName>
     <definedName name="OUTPUT.B">Sheet1!$A$3:$U$3</definedName>
@@ -28,11 +30,7 @@
     <definedName name="X_values">Sheet1!$A$1:$U$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -41,6 +39,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -48,6 +49,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
+    <t>Factor</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
     <t>Webtool Page</t>
   </si>
   <si>
@@ -66,55 +73,49 @@
     <t>Named Range</t>
   </si>
   <si>
+    <t>Graph Type</t>
+  </si>
+  <si>
+    <t>Y axis min</t>
+  </si>
+  <si>
+    <t>Y axis max</t>
+  </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
+    <t>tab one</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>First output</t>
+  </si>
+  <si>
     <t>No Units</t>
   </si>
   <si>
-    <t>Overview</t>
-  </si>
-  <si>
-    <t>Top</t>
+    <t>output.A</t>
+  </si>
+  <si>
+    <t>Line</t>
+  </si>
+  <si>
+    <t>Stacked Area with overlying Line(s)</t>
   </si>
   <si>
     <t>Bottom</t>
   </si>
   <si>
+    <t>Second output</t>
+  </si>
+  <si>
     <t>TWh/yr</t>
   </si>
   <si>
-    <t>Graph Type</t>
-  </si>
-  <si>
-    <t>Y axis min</t>
-  </si>
-  <si>
-    <t>Y axis max</t>
-  </si>
-  <si>
-    <t>Stacked Area with overlying Line(s)</t>
-  </si>
-  <si>
-    <t>Line</t>
-  </si>
-  <si>
-    <t>output.A</t>
-  </si>
-  <si>
     <t>output.B</t>
-  </si>
-  <si>
-    <t>tab one</t>
-  </si>
-  <si>
-    <t>First output</t>
-  </si>
-  <si>
-    <t>Second output</t>
-  </si>
-  <si>
-    <t>Factor</t>
-  </si>
-  <si>
-    <t>Offset</t>
   </si>
 </sst>
 </file>
@@ -124,10 +125,10 @@
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -465,16 +466,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE10450A-E94A-4F5E-8BAC-3DBE686CA3F0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -544,312 +545,327 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>X_values*INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values*INPUT.FACTOR+INPUT.OFFSET+Control!$C1-Control!$D1</f>
         <v>1</v>
       </c>
       <c r="B2">
-        <f>X_values*INPUT.FACTOR+INPUT.OFFSET</f>
-        <v>1.2</v>
+        <f>X_values*INPUT.FACTOR+INPUT.OFFSET+Control!$C1-Control!$D1</f>
+        <v>1.2000000000000002</v>
       </c>
       <c r="C2">
-        <f>X_values*INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values*INPUT.FACTOR+INPUT.OFFSET+Control!$C1-Control!$D1</f>
         <v>1.4</v>
       </c>
       <c r="D2">
-        <f>X_values*INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values*INPUT.FACTOR+INPUT.OFFSET+Control!$C1-Control!$D1</f>
         <v>1.6</v>
       </c>
       <c r="E2">
-        <f>X_values*INPUT.FACTOR+INPUT.OFFSET</f>
-        <v>1.8</v>
+        <f>X_values*INPUT.FACTOR+INPUT.OFFSET+Control!$C1-Control!$D1</f>
+        <v>1.7999999999999998</v>
       </c>
       <c r="F2">
-        <f>X_values*INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values*INPUT.FACTOR+INPUT.OFFSET+Control!$C1-Control!$D1</f>
         <v>2</v>
       </c>
       <c r="G2">
-        <f>X_values*INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values*INPUT.FACTOR+INPUT.OFFSET+Control!$C1-Control!$D1</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="H2">
-        <f>X_values*INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values*INPUT.FACTOR+INPUT.OFFSET+Control!$C1-Control!$D1</f>
         <v>2.4</v>
       </c>
       <c r="I2">
-        <f>X_values*INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values*INPUT.FACTOR+INPUT.OFFSET+Control!$C1-Control!$D1</f>
         <v>2.6</v>
       </c>
       <c r="J2">
-        <f>X_values*INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values*INPUT.FACTOR+INPUT.OFFSET+Control!$C1-Control!$D1</f>
         <v>2.8</v>
       </c>
       <c r="K2">
-        <f>X_values*INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values*INPUT.FACTOR+INPUT.OFFSET+Control!$C1-Control!$D1</f>
         <v>3</v>
       </c>
       <c r="L2">
-        <f>X_values*INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values*INPUT.FACTOR+INPUT.OFFSET+Control!$C1-Control!$D1</f>
         <v>3.2</v>
       </c>
       <c r="M2">
-        <f>X_values*INPUT.FACTOR+INPUT.OFFSET</f>
-        <v>3.4</v>
+        <f>X_values*INPUT.FACTOR+INPUT.OFFSET+Control!$C1-Control!$D1</f>
+        <v>3.4000000000000004</v>
       </c>
       <c r="N2">
-        <f>X_values*INPUT.FACTOR+INPUT.OFFSET</f>
-        <v>3.6</v>
+        <f>X_values*INPUT.FACTOR+INPUT.OFFSET+Control!$C1-Control!$D1</f>
+        <v>3.5999999999999996</v>
       </c>
       <c r="O2">
-        <f>X_values*INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values*INPUT.FACTOR+INPUT.OFFSET+Control!$C1-Control!$D1</f>
         <v>3.8</v>
       </c>
       <c r="P2">
-        <f>X_values*INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values*INPUT.FACTOR+INPUT.OFFSET+Control!$C1-Control!$D1</f>
         <v>4</v>
       </c>
       <c r="Q2">
-        <f>X_values*INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values*INPUT.FACTOR+INPUT.OFFSET+Control!$C1-Control!$D1</f>
         <v>4.2</v>
       </c>
       <c r="R2">
-        <f>X_values*INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values*INPUT.FACTOR+INPUT.OFFSET+Control!$C1-Control!$D1</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="S2">
-        <f>X_values*INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values*INPUT.FACTOR+INPUT.OFFSET+Control!$C1-Control!$D1</f>
         <v>4.5999999999999996</v>
       </c>
       <c r="T2">
-        <f>X_values*INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values*INPUT.FACTOR+INPUT.OFFSET+Control!$C1-Control!$D1</f>
         <v>4.8</v>
       </c>
       <c r="U2">
-        <f>X_values*INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values*INPUT.FACTOR+INPUT.OFFSET+Control!$C1-Control!$D1</f>
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>X_values^INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values^INPUT.FACTOR+INPUT.OFFSET+Control!$C2-Control!$D2</f>
         <v>1</v>
       </c>
       <c r="B3">
-        <f>X_values^INPUT.FACTOR+INPUT.OFFSET</f>
-        <v>1.01</v>
+        <f>X_values^INPUT.FACTOR+INPUT.OFFSET+Control!$C2-Control!$D2</f>
+        <v>1.0099999999999998</v>
       </c>
       <c r="C3">
-        <f>X_values^INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values^INPUT.FACTOR+INPUT.OFFSET+Control!$C2-Control!$D2</f>
         <v>1.04</v>
       </c>
       <c r="D3">
-        <f>X_values^INPUT.FACTOR+INPUT.OFFSET</f>
-        <v>1.0900000000000001</v>
+        <f>X_values^INPUT.FACTOR+INPUT.OFFSET+Control!$C2-Control!$D2</f>
+        <v>1.0899999999999999</v>
       </c>
       <c r="E3">
-        <f>X_values^INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values^INPUT.FACTOR+INPUT.OFFSET+Control!$C2-Control!$D2</f>
         <v>1.1600000000000001</v>
       </c>
       <c r="F3">
-        <f>X_values^INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values^INPUT.FACTOR+INPUT.OFFSET+Control!$C2-Control!$D2</f>
         <v>1.25</v>
       </c>
       <c r="G3">
-        <f>X_values^INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values^INPUT.FACTOR+INPUT.OFFSET+Control!$C2-Control!$D2</f>
         <v>1.3599999999999999</v>
       </c>
       <c r="H3">
-        <f>X_values^INPUT.FACTOR+INPUT.OFFSET</f>
-        <v>1.49</v>
+        <f>X_values^INPUT.FACTOR+INPUT.OFFSET+Control!$C2-Control!$D2</f>
+        <v>1.4900000000000002</v>
       </c>
       <c r="I3">
-        <f>X_values^INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values^INPUT.FACTOR+INPUT.OFFSET+Control!$C2-Control!$D2</f>
         <v>1.6400000000000001</v>
       </c>
       <c r="J3">
-        <f>X_values^INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values^INPUT.FACTOR+INPUT.OFFSET+Control!$C2-Control!$D2</f>
         <v>1.81</v>
       </c>
       <c r="K3">
-        <f>X_values^INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values^INPUT.FACTOR+INPUT.OFFSET+Control!$C2-Control!$D2</f>
         <v>2</v>
       </c>
       <c r="L3">
-        <f>X_values^INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values^INPUT.FACTOR+INPUT.OFFSET+Control!$C2-Control!$D2</f>
         <v>2.21</v>
       </c>
       <c r="M3">
-        <f>X_values^INPUT.FACTOR+INPUT.OFFSET</f>
-        <v>2.44</v>
+        <f>X_values^INPUT.FACTOR+INPUT.OFFSET+Control!$C2-Control!$D2</f>
+        <v>2.4399999999999995</v>
       </c>
       <c r="N3">
-        <f>X_values^INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values^INPUT.FACTOR+INPUT.OFFSET+Control!$C2-Control!$D2</f>
         <v>2.6900000000000004</v>
       </c>
       <c r="O3">
-        <f>X_values^INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values^INPUT.FACTOR+INPUT.OFFSET+Control!$C2-Control!$D2</f>
         <v>2.96</v>
       </c>
       <c r="P3">
-        <f>X_values^INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values^INPUT.FACTOR+INPUT.OFFSET+Control!$C2-Control!$D2</f>
         <v>3.25</v>
       </c>
       <c r="Q3">
-        <f>X_values^INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values^INPUT.FACTOR+INPUT.OFFSET+Control!$C2-Control!$D2</f>
         <v>3.5600000000000005</v>
       </c>
       <c r="R3">
-        <f>X_values^INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values^INPUT.FACTOR+INPUT.OFFSET+Control!$C2-Control!$D2</f>
         <v>3.8899999999999997</v>
       </c>
       <c r="S3">
-        <f>X_values^INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values^INPUT.FACTOR+INPUT.OFFSET+Control!$C2-Control!$D2</f>
         <v>4.24</v>
       </c>
       <c r="T3">
-        <f>X_values^INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values^INPUT.FACTOR+INPUT.OFFSET+Control!$C2-Control!$D2</f>
         <v>4.6099999999999994</v>
       </c>
       <c r="U3">
-        <f>X_values^INPUT.FACTOR+INPUT.OFFSET</f>
+        <f>X_values^INPUT.FACTOR+INPUT.OFFSET+Control!$C2-Control!$D2</f>
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18BF4404-6867-44D0-A30D-5CE90D68DC55}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B1">
         <v>2</v>
       </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E30DA4FD-6713-4A4E-B223-E53DB68B8B14}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="43.5703125" customWidth="1"/>
+    <col min="7" max="7" width="33.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>